<commit_message>
updated data.xlsx in baselines
Added fuel2 and efficiency2 to data sheet. Updated code in NETS and LDS to run certain scenarios.
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/long_duration_storage/data/monte_carlo_inputs.xlsx
+++ b/projects/va_emerging_tech/long_duration_storage/data/monte_carlo_inputs.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F756528-2E08-4081-9EAC-A299FED87E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3AB34C-E799-4CF1-9C45-9E8ED75649F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lowBio" sheetId="12" r:id="rId1"/>
     <sheet name="highBio" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>uniform</t>
   </si>
@@ -74,12 +83,6 @@
     <t>EC_DAC</t>
   </si>
   <si>
-    <t>EC_VFB</t>
-  </si>
-  <si>
-    <t>Lower: Bennett et al., Upper: Mouli-Castillo</t>
-  </si>
-  <si>
     <t>Fuels</t>
   </si>
   <si>
@@ -92,13 +95,7 @@
     <t>[PJ]</t>
   </si>
   <si>
-    <t>Lower: Li et al 10 hr, Upper: Beuse et al.</t>
-  </si>
-  <si>
     <t>Keith et al. early plant and Nth plant</t>
-  </si>
-  <si>
-    <t>EC_OCAES</t>
   </si>
   <si>
     <t>Lower: NETL Vol 2 &amp; Upper: Fajardy et al.</t>
@@ -444,23 +441,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C088720-46C9-4463-BD2A-99BFD76A219D}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1015625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.68359375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -492,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -519,10 +516,10 @@
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -549,88 +546,44 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1457</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>52.6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>1457</v>
+        <v>52.6</v>
       </c>
       <c r="H4" s="1">
-        <v>9191</v>
+        <v>105.2</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4317</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1820</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3781</v>
-      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>52.6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
+      <c r="J5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -639,23 +592,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F9DF2A-4D9C-45A5-87BB-AF98F5BFA577}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1015625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.68359375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -687,7 +640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -714,10 +667,10 @@
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -731,7 +684,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="1">
-        <v>2562</v>
+        <v>3704</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>0</v>
@@ -744,89 +697,42 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1457</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>105.2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>1457</v>
+        <v>52.6</v>
       </c>
       <c r="H4" s="1">
-        <v>9191</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4317</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1820</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3781</v>
-      </c>
+        <v>105.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <f>52.6*2</f>
-        <v>105.2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
+      <c r="J5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>